<commit_message>
Update index.html via workflow
</commit_message>
<xml_diff>
--- a/ofsted_csc_ilacs_overview.xlsx
+++ b/ofsted_csc_ilacs_overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2921" uniqueCount="1424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2921" uniqueCount="1423">
   <si>
     <t>80426</t>
   </si>
@@ -1039,7 +1039,7 @@
     <t>372, 370, 384, 894, 357, 812, 335, 861, 354, 813</t>
   </si>
   <si>
-    <t>[(372, 'good'), (370, 'good'), (384, 'good'), (894, 'outstanding'), (357, 'inadequate'), (812, 'inadequate'), (335, 'outstanding'), (861, 'requires improvement'), (354, 'requires improvement'), (813, 'outstanding')]</t>
+    <t>[(372, 'good'), (370, 'good'), (384, 'good'), (894, 'outstanding'), (357, 'inadequate'), (812, 'good'), (335, 'outstanding'), (861, 'requires improvement'), (354, 'requires improvement'), (813, 'outstanding')]</t>
   </si>
   <si>
     <t>doncaster</t>
@@ -1504,7 +1504,7 @@
     <t>333, 336, 861, 335, 812, 354, 806, 371, 831, 372</t>
   </si>
   <si>
-    <t>[(333, 'requires improvement'), (336, 'good'), (861, 'requires improvement'), (335, 'outstanding'), (812, 'inadequate'), (354, 'requires improvement'), (806, 'requires improvement'), (371, 'good'), (831, 'outstanding'), (372, 'good')]</t>
+    <t>[(333, 'requires improvement'), (336, 'good'), (861, 'requires improvement'), (335, 'outstanding'), (812, 'good'), (354, 'requires improvement'), (806, 'requires improvement'), (371, 'good'), (831, 'outstanding'), (372, 'good')]</t>
   </si>
   <si>
     <t>kingston upon hull</t>
@@ -2746,16 +2746,13 @@
     <t>north east lincolnshire</t>
   </si>
   <si>
-    <t>https://files.ofsted.gov.uk/v1/file/50172853</t>
-  </si>
-  <si>
-    <t>04/10/2021</t>
-  </si>
-  <si>
-    <t>15/10/2021</t>
-  </si>
-  <si>
-    <t>26/11/21</t>
+    <t>https://files.ofsted.gov.uk/v1/file/50285393</t>
+  </si>
+  <si>
+    <t>25/07/2025</t>
+  </si>
+  <si>
+    <t>03/09/25</t>
   </si>
   <si>
     <t>80527</t>
@@ -3682,7 +3679,7 @@
     <t>335, 354, 336, 371, 812, 810, 333, 357, 831, 372</t>
   </si>
   <si>
-    <t>[(335, 'outstanding'), (354, 'requires improvement'), (336, 'good'), (371, 'good'), (812, 'inadequate'), (810, 'requires improvement'), (333, 'requires improvement'), (357, 'inadequate'), (831, 'outstanding'), (372, 'good')]</t>
+    <t>[(335, 'outstanding'), (354, 'requires improvement'), (336, 'good'), (371, 'good'), (812, 'good'), (810, 'requires improvement'), (333, 'requires improvement'), (357, 'inadequate'), (831, 'outstanding'), (372, 'good')]</t>
   </si>
   <si>
     <t>stoke-on-trent</t>
@@ -3919,7 +3916,7 @@
     <t>354, 861, 357, 336, 371, 831, 350, 372, 812, 333</t>
   </si>
   <si>
-    <t>[(354, 'requires improvement'), (861, 'requires improvement'), (357, 'inadequate'), (336, 'good'), (371, 'good'), (831, 'outstanding'), (350, 'good'), (372, 'good'), (812, 'inadequate'), (333, 'requires improvement')]</t>
+    <t>[(354, 'requires improvement'), (861, 'requires improvement'), (357, 'inadequate'), (336, 'good'), (371, 'good'), (831, 'outstanding'), (350, 'good'), (372, 'good'), (812, 'good'), (333, 'requires improvement')]</t>
   </si>
   <si>
     <t>walsall</t>
@@ -4189,7 +4186,7 @@
     <t>333, 861, 335, 810, 354, 331, 371, 831, 806, 812</t>
   </si>
   <si>
-    <t>[(333, 'requires improvement'), (861, 'requires improvement'), (335, 'outstanding'), (810, 'requires improvement'), (354, 'requires improvement'), (331, 'good'), (371, 'good'), (831, 'outstanding'), (806, 'requires improvement'), (812, 'inadequate')]</t>
+    <t>[(333, 'requires improvement'), (861, 'requires improvement'), (335, 'outstanding'), (810, 'requires improvement'), (354, 'requires improvement'), (331, 'good'), (371, 'good'), (831, 'outstanding'), (806, 'requires improvement'), (812, 'good')]</t>
   </si>
   <si>
     <t>wolverhampton</t>
@@ -4656,64 +4653,64 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1404</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1405</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1406</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1407</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1408</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1409</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1410</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1411</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>1412</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>1413</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>1414</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>1415</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>1416</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>1417</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>1418</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>1419</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>1420</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>1421</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>1422</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>1423</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -5904,7 +5901,7 @@
         <v>78</v>
       </c>
       <c r="T20" t="s">
-        <v>66</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -6849,7 +6846,7 @@
         <v>106</v>
       </c>
       <c r="T35" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -8046,7 +8043,7 @@
         <v>106</v>
       </c>
       <c r="T54" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:20">
@@ -10532,67 +10529,67 @@
         <v>910</v>
       </c>
       <c r="I94" t="s">
-        <v>191</v>
+        <v>8</v>
       </c>
       <c r="J94" t="s">
         <v>48</v>
       </c>
       <c r="K94" t="s">
-        <v>213</v>
+        <v>375</v>
       </c>
       <c r="L94" t="s">
+        <v>37</v>
+      </c>
+      <c r="M94" t="s">
         <v>911</v>
       </c>
-      <c r="M94" t="s">
+      <c r="N94" t="s">
         <v>912</v>
-      </c>
-      <c r="N94" t="s">
-        <v>913</v>
       </c>
       <c r="O94" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80526_north east lincolnshire", ".\export_data\inspection_reports\80526_north east lincolnshire")</f>
         <v>0</v>
       </c>
       <c r="P94" t="s">
-        <v>191</v>
+        <v>106</v>
       </c>
       <c r="Q94" t="s">
-        <v>191</v>
+        <v>8</v>
       </c>
       <c r="R94" t="s">
-        <v>191</v>
+        <v>8</v>
       </c>
       <c r="S94" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="T94" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
     </row>
     <row r="95" spans="1:20">
       <c r="A95" t="s">
+        <v>913</v>
+      </c>
+      <c r="B95" t="s">
         <v>914</v>
-      </c>
-      <c r="B95" t="s">
-        <v>915</v>
       </c>
       <c r="C95" t="s">
         <v>2</v>
       </c>
       <c r="D95" t="s">
+        <v>915</v>
+      </c>
+      <c r="E95" t="s">
         <v>916</v>
       </c>
-      <c r="E95" t="s">
+      <c r="F95" t="s">
         <v>917</v>
       </c>
-      <c r="F95" t="s">
+      <c r="G95" t="s">
         <v>918</v>
       </c>
-      <c r="G95" t="s">
+      <c r="H95" s="2" t="s">
         <v>919</v>
-      </c>
-      <c r="H95" s="2" t="s">
-        <v>920</v>
       </c>
       <c r="I95" t="s">
         <v>106</v>
@@ -10601,16 +10598,16 @@
         <v>9</v>
       </c>
       <c r="K95" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="L95" t="s">
         <v>301</v>
       </c>
       <c r="M95" t="s">
+        <v>921</v>
+      </c>
+      <c r="N95" t="s">
         <v>922</v>
-      </c>
-      <c r="N95" t="s">
-        <v>923</v>
       </c>
       <c r="O95" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80527_north lincolnshire", ".\export_data\inspection_reports\80527_north lincolnshire")</f>
@@ -10634,28 +10631,28 @@
     </row>
     <row r="96" spans="1:20">
       <c r="A96" t="s">
+        <v>923</v>
+      </c>
+      <c r="B96" t="s">
         <v>924</v>
-      </c>
-      <c r="B96" t="s">
-        <v>925</v>
       </c>
       <c r="C96" t="s">
         <v>306</v>
       </c>
       <c r="D96" t="s">
+        <v>925</v>
+      </c>
+      <c r="E96" t="s">
         <v>926</v>
       </c>
-      <c r="E96" t="s">
+      <c r="F96" t="s">
         <v>927</v>
       </c>
-      <c r="F96" t="s">
+      <c r="G96" t="s">
         <v>928</v>
       </c>
-      <c r="G96" t="s">
+      <c r="H96" s="2" t="s">
         <v>929</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>930</v>
       </c>
       <c r="I96" t="s">
         <v>14</v>
@@ -10667,13 +10664,13 @@
         <v>202</v>
       </c>
       <c r="L96" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="M96" t="s">
+        <v>921</v>
+      </c>
+      <c r="N96" t="s">
         <v>922</v>
-      </c>
-      <c r="N96" t="s">
-        <v>923</v>
       </c>
       <c r="O96" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\2637539_north northamptonshire", ".\export_data\inspection_reports\2637539_north northamptonshire")</f>
@@ -10697,28 +10694,28 @@
     </row>
     <row r="97" spans="1:20">
       <c r="A97" t="s">
+        <v>931</v>
+      </c>
+      <c r="B97" t="s">
         <v>932</v>
-      </c>
-      <c r="B97" t="s">
-        <v>933</v>
       </c>
       <c r="C97" t="s">
         <v>18</v>
       </c>
       <c r="D97" t="s">
+        <v>933</v>
+      </c>
+      <c r="E97" t="s">
         <v>934</v>
       </c>
-      <c r="E97" t="s">
+      <c r="F97" t="s">
         <v>935</v>
       </c>
-      <c r="F97" t="s">
+      <c r="G97" t="s">
         <v>936</v>
       </c>
-      <c r="G97" t="s">
+      <c r="H97" s="2" t="s">
         <v>937</v>
-      </c>
-      <c r="H97" s="2" t="s">
-        <v>938</v>
       </c>
       <c r="I97" t="s">
         <v>14</v>
@@ -10736,7 +10733,7 @@
         <v>576</v>
       </c>
       <c r="N97" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="O97" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80528_north somerset", ".\export_data\inspection_reports\80528_north somerset")</f>
@@ -10760,28 +10757,28 @@
     </row>
     <row r="98" spans="1:20">
       <c r="A98" t="s">
+        <v>939</v>
+      </c>
+      <c r="B98" t="s">
         <v>940</v>
-      </c>
-      <c r="B98" t="s">
-        <v>941</v>
       </c>
       <c r="C98" t="s">
         <v>294</v>
       </c>
       <c r="D98" t="s">
+        <v>941</v>
+      </c>
+      <c r="E98" t="s">
         <v>942</v>
       </c>
-      <c r="E98" t="s">
+      <c r="F98" t="s">
         <v>943</v>
       </c>
-      <c r="F98" t="s">
+      <c r="G98" t="s">
         <v>944</v>
       </c>
-      <c r="G98" t="s">
+      <c r="H98" s="2" t="s">
         <v>945</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>946</v>
       </c>
       <c r="I98" t="s">
         <v>106</v>
@@ -10818,33 +10815,33 @@
         <v>106</v>
       </c>
       <c r="T98" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
     </row>
     <row r="99" spans="1:20">
       <c r="A99" t="s">
+        <v>946</v>
+      </c>
+      <c r="B99" t="s">
         <v>947</v>
-      </c>
-      <c r="B99" t="s">
-        <v>948</v>
       </c>
       <c r="C99" t="s">
         <v>2</v>
       </c>
       <c r="D99" t="s">
+        <v>948</v>
+      </c>
+      <c r="E99" t="s">
         <v>949</v>
       </c>
-      <c r="E99" t="s">
+      <c r="F99" t="s">
         <v>950</v>
       </c>
-      <c r="F99" t="s">
+      <c r="G99" t="s">
         <v>951</v>
       </c>
-      <c r="G99" t="s">
+      <c r="H99" s="2" t="s">
         <v>952</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>953</v>
       </c>
       <c r="I99" t="s">
         <v>106</v>
@@ -10853,16 +10850,16 @@
         <v>9</v>
       </c>
       <c r="K99" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="L99" t="s">
+        <v>953</v>
+      </c>
+      <c r="M99" t="s">
         <v>954</v>
       </c>
-      <c r="M99" t="s">
+      <c r="N99" t="s">
         <v>955</v>
-      </c>
-      <c r="N99" t="s">
-        <v>956</v>
       </c>
       <c r="O99" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80530_north yorkshire", ".\export_data\inspection_reports\80530_north yorkshire")</f>
@@ -10886,28 +10883,28 @@
     </row>
     <row r="100" spans="1:20">
       <c r="A100" t="s">
+        <v>956</v>
+      </c>
+      <c r="B100" t="s">
         <v>957</v>
-      </c>
-      <c r="B100" t="s">
-        <v>958</v>
       </c>
       <c r="C100" t="s">
         <v>294</v>
       </c>
       <c r="D100" t="s">
+        <v>958</v>
+      </c>
+      <c r="E100" t="s">
         <v>959</v>
       </c>
-      <c r="E100" t="s">
+      <c r="F100" t="s">
         <v>960</v>
       </c>
-      <c r="F100" t="s">
+      <c r="G100" t="s">
         <v>961</v>
       </c>
-      <c r="G100" t="s">
+      <c r="H100" s="2" t="s">
         <v>962</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>963</v>
       </c>
       <c r="I100" t="s">
         <v>106</v>
@@ -10916,10 +10913,10 @@
         <v>9</v>
       </c>
       <c r="K100" t="s">
+        <v>963</v>
+      </c>
+      <c r="L100" t="s">
         <v>964</v>
-      </c>
-      <c r="L100" t="s">
-        <v>965</v>
       </c>
       <c r="M100" t="s">
         <v>434</v>
@@ -10949,28 +10946,28 @@
     </row>
     <row r="101" spans="1:20">
       <c r="A101" t="s">
+        <v>965</v>
+      </c>
+      <c r="B101" t="s">
         <v>966</v>
-      </c>
-      <c r="B101" t="s">
-        <v>967</v>
       </c>
       <c r="C101" t="s">
         <v>306</v>
       </c>
       <c r="D101" t="s">
+        <v>967</v>
+      </c>
+      <c r="E101" t="s">
         <v>968</v>
       </c>
-      <c r="E101" t="s">
+      <c r="F101" t="s">
         <v>969</v>
       </c>
-      <c r="F101" t="s">
+      <c r="G101" t="s">
         <v>970</v>
       </c>
-      <c r="G101" t="s">
+      <c r="H101" s="2" t="s">
         <v>971</v>
-      </c>
-      <c r="H101" s="2" t="s">
-        <v>972</v>
       </c>
       <c r="I101" t="s">
         <v>191</v>
@@ -10979,7 +10976,7 @@
         <v>117</v>
       </c>
       <c r="K101" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="N101" t="s">
         <v>847</v>
@@ -11006,28 +11003,28 @@
     </row>
     <row r="102" spans="1:20">
       <c r="A102" t="s">
+        <v>972</v>
+      </c>
+      <c r="B102" t="s">
         <v>973</v>
-      </c>
-      <c r="B102" t="s">
-        <v>974</v>
       </c>
       <c r="C102" t="s">
         <v>306</v>
       </c>
       <c r="D102" t="s">
+        <v>974</v>
+      </c>
+      <c r="E102" t="s">
         <v>975</v>
       </c>
-      <c r="E102" t="s">
+      <c r="F102" t="s">
         <v>976</v>
       </c>
-      <c r="F102" t="s">
+      <c r="G102" t="s">
         <v>977</v>
       </c>
-      <c r="G102" t="s">
+      <c r="H102" s="2" t="s">
         <v>978</v>
-      </c>
-      <c r="H102" s="2" t="s">
-        <v>979</v>
       </c>
       <c r="I102" t="s">
         <v>8</v>
@@ -11039,7 +11036,7 @@
         <v>754</v>
       </c>
       <c r="L102" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="M102" t="s">
         <v>434</v>
@@ -11069,28 +11066,28 @@
     </row>
     <row r="103" spans="1:20">
       <c r="A103" t="s">
+        <v>979</v>
+      </c>
+      <c r="B103" t="s">
         <v>980</v>
-      </c>
-      <c r="B103" t="s">
-        <v>981</v>
       </c>
       <c r="C103" t="s">
         <v>56</v>
       </c>
       <c r="D103" t="s">
+        <v>981</v>
+      </c>
+      <c r="E103" t="s">
         <v>982</v>
       </c>
-      <c r="E103" t="s">
+      <c r="F103" t="s">
         <v>983</v>
       </c>
-      <c r="F103" t="s">
+      <c r="G103" t="s">
         <v>984</v>
       </c>
-      <c r="G103" t="s">
+      <c r="H103" s="2" t="s">
         <v>985</v>
-      </c>
-      <c r="H103" s="2" t="s">
-        <v>986</v>
       </c>
       <c r="I103" t="s">
         <v>8</v>
@@ -11132,28 +11129,28 @@
     </row>
     <row r="104" spans="1:20">
       <c r="A104" t="s">
+        <v>986</v>
+      </c>
+      <c r="B104" t="s">
         <v>987</v>
-      </c>
-      <c r="B104" t="s">
-        <v>988</v>
       </c>
       <c r="C104" t="s">
         <v>100</v>
       </c>
       <c r="D104" t="s">
+        <v>988</v>
+      </c>
+      <c r="E104" t="s">
         <v>989</v>
       </c>
-      <c r="E104" t="s">
+      <c r="F104" t="s">
         <v>990</v>
       </c>
-      <c r="F104" t="s">
+      <c r="G104" t="s">
         <v>991</v>
       </c>
-      <c r="G104" t="s">
+      <c r="H104" s="2" t="s">
         <v>992</v>
-      </c>
-      <c r="H104" s="2" t="s">
-        <v>993</v>
       </c>
       <c r="I104" t="s">
         <v>8</v>
@@ -11165,13 +11162,13 @@
         <v>754</v>
       </c>
       <c r="L104" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="M104" t="s">
         <v>163</v>
       </c>
       <c r="N104" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="O104" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80536_oxfordshire", ".\export_data\inspection_reports\80536_oxfordshire")</f>
@@ -11195,28 +11192,28 @@
     </row>
     <row r="105" spans="1:20">
       <c r="A105" t="s">
+        <v>995</v>
+      </c>
+      <c r="B105" t="s">
         <v>996</v>
-      </c>
-      <c r="B105" t="s">
-        <v>997</v>
       </c>
       <c r="C105" t="s">
         <v>31</v>
       </c>
       <c r="D105" t="s">
+        <v>997</v>
+      </c>
+      <c r="E105" t="s">
         <v>998</v>
       </c>
-      <c r="E105" t="s">
+      <c r="F105" t="s">
         <v>999</v>
       </c>
-      <c r="F105" t="s">
+      <c r="G105" t="s">
         <v>1000</v>
       </c>
-      <c r="G105" t="s">
+      <c r="H105" s="2" t="s">
         <v>1001</v>
-      </c>
-      <c r="H105" s="2" t="s">
-        <v>1002</v>
       </c>
       <c r="I105" t="s">
         <v>191</v>
@@ -11228,13 +11225,13 @@
         <v>743</v>
       </c>
       <c r="L105" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M105" t="s">
         <v>1003</v>
       </c>
-      <c r="M105" t="s">
+      <c r="N105" t="s">
         <v>1004</v>
-      </c>
-      <c r="N105" t="s">
-        <v>1005</v>
       </c>
       <c r="O105" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80537_peterborough", ".\export_data\inspection_reports\80537_peterborough")</f>
@@ -11258,28 +11255,28 @@
     </row>
     <row r="106" spans="1:20">
       <c r="A106" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B106" t="s">
         <v>1006</v>
-      </c>
-      <c r="B106" t="s">
-        <v>1007</v>
       </c>
       <c r="C106" t="s">
         <v>18</v>
       </c>
       <c r="D106" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E106" t="s">
         <v>1008</v>
       </c>
-      <c r="E106" t="s">
+      <c r="F106" t="s">
         <v>1009</v>
       </c>
-      <c r="F106" t="s">
+      <c r="G106" t="s">
         <v>1010</v>
       </c>
-      <c r="G106" t="s">
+      <c r="H106" s="2" t="s">
         <v>1011</v>
-      </c>
-      <c r="H106" s="2" t="s">
-        <v>1012</v>
       </c>
       <c r="I106" t="s">
         <v>14</v>
@@ -11291,13 +11288,13 @@
         <v>127</v>
       </c>
       <c r="L106" t="s">
+        <v>1012</v>
+      </c>
+      <c r="M106" t="s">
         <v>1013</v>
       </c>
-      <c r="M106" t="s">
+      <c r="N106" t="s">
         <v>1014</v>
-      </c>
-      <c r="N106" t="s">
-        <v>1015</v>
       </c>
       <c r="O106" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80538_plymouth", ".\export_data\inspection_reports\80538_plymouth")</f>
@@ -11321,28 +11318,28 @@
     </row>
     <row r="107" spans="1:20">
       <c r="A107" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B107" t="s">
         <v>1016</v>
-      </c>
-      <c r="B107" t="s">
-        <v>1017</v>
       </c>
       <c r="C107" t="s">
         <v>100</v>
       </c>
       <c r="D107" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E107" t="s">
         <v>1018</v>
       </c>
-      <c r="E107" t="s">
+      <c r="F107" t="s">
         <v>1019</v>
       </c>
-      <c r="F107" t="s">
+      <c r="G107" t="s">
         <v>1020</v>
       </c>
-      <c r="G107" t="s">
+      <c r="H107" s="2" t="s">
         <v>1021</v>
-      </c>
-      <c r="H107" s="2" t="s">
-        <v>1022</v>
       </c>
       <c r="I107" t="s">
         <v>8</v>
@@ -11354,13 +11351,13 @@
         <v>225</v>
       </c>
       <c r="L107" t="s">
+        <v>1022</v>
+      </c>
+      <c r="M107" t="s">
         <v>1023</v>
       </c>
-      <c r="M107" t="s">
+      <c r="N107" t="s">
         <v>1024</v>
-      </c>
-      <c r="N107" t="s">
-        <v>1025</v>
       </c>
       <c r="O107" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80539_portsmouth", ".\export_data\inspection_reports\80539_portsmouth")</f>
@@ -11384,28 +11381,28 @@
     </row>
     <row r="108" spans="1:20">
       <c r="A108" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B108" t="s">
         <v>1026</v>
-      </c>
-      <c r="B108" t="s">
-        <v>1027</v>
       </c>
       <c r="C108" t="s">
         <v>100</v>
       </c>
       <c r="D108" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E108" t="s">
         <v>1028</v>
       </c>
-      <c r="E108" t="s">
+      <c r="F108" t="s">
         <v>1029</v>
       </c>
-      <c r="F108" t="s">
+      <c r="G108" t="s">
         <v>1030</v>
       </c>
-      <c r="G108" t="s">
+      <c r="H108" s="2" t="s">
         <v>1031</v>
-      </c>
-      <c r="H108" s="2" t="s">
-        <v>1032</v>
       </c>
       <c r="I108" t="s">
         <v>14</v>
@@ -11447,28 +11444,28 @@
     </row>
     <row r="109" spans="1:20">
       <c r="A109" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B109" t="s">
         <v>1033</v>
-      </c>
-      <c r="B109" t="s">
-        <v>1034</v>
       </c>
       <c r="C109" t="s">
         <v>294</v>
       </c>
       <c r="D109" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E109" t="s">
         <v>1035</v>
       </c>
-      <c r="E109" t="s">
+      <c r="F109" t="s">
         <v>1036</v>
       </c>
-      <c r="F109" t="s">
+      <c r="G109" t="s">
         <v>1037</v>
       </c>
-      <c r="G109" t="s">
+      <c r="H109" s="2" t="s">
         <v>1038</v>
-      </c>
-      <c r="H109" s="2" t="s">
-        <v>1039</v>
       </c>
       <c r="I109" t="s">
         <v>14</v>
@@ -11477,10 +11474,10 @@
         <v>117</v>
       </c>
       <c r="K109" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="N109" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="O109" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80541_redcar and cleveland", ".\export_data\inspection_reports\80541_redcar and cleveland")</f>
@@ -11504,28 +11501,28 @@
     </row>
     <row r="110" spans="1:20">
       <c r="A110" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B110" t="s">
         <v>1041</v>
-      </c>
-      <c r="B110" t="s">
-        <v>1042</v>
       </c>
       <c r="C110" t="s">
         <v>56</v>
       </c>
       <c r="D110" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E110" t="s">
         <v>1043</v>
       </c>
-      <c r="E110" t="s">
+      <c r="F110" t="s">
         <v>1044</v>
       </c>
-      <c r="F110" t="s">
+      <c r="G110" t="s">
         <v>1045</v>
       </c>
-      <c r="G110" t="s">
+      <c r="H110" s="2" t="s">
         <v>1046</v>
-      </c>
-      <c r="H110" s="2" t="s">
-        <v>1047</v>
       </c>
       <c r="I110" t="s">
         <v>14</v>
@@ -11540,10 +11537,10 @@
         <v>472</v>
       </c>
       <c r="M110" t="s">
+        <v>1047</v>
+      </c>
+      <c r="N110" t="s">
         <v>1048</v>
-      </c>
-      <c r="N110" t="s">
-        <v>1049</v>
       </c>
       <c r="O110" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80542_rochdale", ".\export_data\inspection_reports\80542_rochdale")</f>
@@ -11567,28 +11564,28 @@
     </row>
     <row r="111" spans="1:20">
       <c r="A111" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B111" t="s">
         <v>1050</v>
-      </c>
-      <c r="B111" t="s">
-        <v>1051</v>
       </c>
       <c r="C111" t="s">
         <v>2</v>
       </c>
       <c r="D111" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E111" t="s">
         <v>1052</v>
       </c>
-      <c r="E111" t="s">
+      <c r="F111" t="s">
         <v>1053</v>
       </c>
-      <c r="F111" t="s">
+      <c r="G111" t="s">
         <v>1054</v>
       </c>
-      <c r="G111" t="s">
+      <c r="H111" s="2" t="s">
         <v>1055</v>
-      </c>
-      <c r="H111" s="2" t="s">
-        <v>1056</v>
       </c>
       <c r="I111" t="s">
         <v>8</v>
@@ -11597,10 +11594,10 @@
         <v>9</v>
       </c>
       <c r="K111" t="s">
+        <v>1056</v>
+      </c>
+      <c r="L111" t="s">
         <v>1057</v>
-      </c>
-      <c r="L111" t="s">
-        <v>1058</v>
       </c>
       <c r="M111" t="s">
         <v>280</v>
@@ -11630,28 +11627,28 @@
     </row>
     <row r="112" spans="1:20">
       <c r="A112" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B112" t="s">
         <v>1059</v>
-      </c>
-      <c r="B112" t="s">
-        <v>1060</v>
       </c>
       <c r="C112" t="s">
         <v>219</v>
       </c>
       <c r="D112" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E112" t="s">
         <v>1061</v>
       </c>
-      <c r="E112" t="s">
+      <c r="F112" t="s">
         <v>1062</v>
       </c>
-      <c r="F112" t="s">
+      <c r="G112" t="s">
         <v>1063</v>
       </c>
-      <c r="G112" t="s">
+      <c r="H112" s="2" t="s">
         <v>1064</v>
-      </c>
-      <c r="H112" s="2" t="s">
-        <v>1065</v>
       </c>
       <c r="I112" t="s">
         <v>106</v>
@@ -11693,28 +11690,28 @@
     </row>
     <row r="113" spans="1:20">
       <c r="A113" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B113" t="s">
         <v>1066</v>
-      </c>
-      <c r="B113" t="s">
-        <v>1067</v>
       </c>
       <c r="C113" t="s">
         <v>219</v>
       </c>
       <c r="D113" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E113" t="s">
         <v>1068</v>
       </c>
-      <c r="E113" t="s">
+      <c r="F113" t="s">
         <v>1069</v>
       </c>
-      <c r="F113" t="s">
+      <c r="G113" t="s">
         <v>1070</v>
       </c>
-      <c r="G113" t="s">
+      <c r="H113" s="2" t="s">
         <v>1071</v>
-      </c>
-      <c r="H113" s="2" t="s">
-        <v>1072</v>
       </c>
       <c r="I113" t="s">
         <v>106</v>
@@ -11756,28 +11753,28 @@
     </row>
     <row r="114" spans="1:20">
       <c r="A114" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B114" t="s">
         <v>1073</v>
-      </c>
-      <c r="B114" t="s">
-        <v>1074</v>
       </c>
       <c r="C114" t="s">
         <v>100</v>
       </c>
       <c r="D114" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E114" t="s">
         <v>1075</v>
       </c>
-      <c r="E114" t="s">
+      <c r="F114" t="s">
         <v>1076</v>
       </c>
-      <c r="F114" t="s">
+      <c r="G114" t="s">
         <v>1077</v>
       </c>
-      <c r="G114" t="s">
+      <c r="H114" s="2" t="s">
         <v>1078</v>
-      </c>
-      <c r="H114" s="2" t="s">
-        <v>1079</v>
       </c>
       <c r="I114" t="s">
         <v>8</v>
@@ -11795,7 +11792,7 @@
         <v>334</v>
       </c>
       <c r="N114" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="O114" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80546_windsor &amp; maidenhead", ".\export_data\inspection_reports\80546_windsor &amp; maidenhead")</f>
@@ -11819,28 +11816,28 @@
     </row>
     <row r="115" spans="1:20">
       <c r="A115" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B115" t="s">
         <v>1081</v>
-      </c>
-      <c r="B115" t="s">
-        <v>1082</v>
       </c>
       <c r="C115" t="s">
         <v>306</v>
       </c>
       <c r="D115" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E115" t="s">
         <v>1083</v>
       </c>
-      <c r="E115" t="s">
+      <c r="F115" t="s">
         <v>1084</v>
       </c>
-      <c r="F115" t="s">
+      <c r="G115" t="s">
         <v>1085</v>
       </c>
-      <c r="G115" t="s">
+      <c r="H115" s="2" t="s">
         <v>1086</v>
-      </c>
-      <c r="H115" s="2" t="s">
-        <v>1087</v>
       </c>
       <c r="I115" t="s">
         <v>8</v>
@@ -11852,10 +11849,10 @@
         <v>509</v>
       </c>
       <c r="L115" t="s">
+        <v>1087</v>
+      </c>
+      <c r="M115" t="s">
         <v>1088</v>
-      </c>
-      <c r="M115" t="s">
-        <v>1089</v>
       </c>
       <c r="N115" t="s">
         <v>435</v>
@@ -11882,28 +11879,28 @@
     </row>
     <row r="116" spans="1:20">
       <c r="A116" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B116" t="s">
         <v>1090</v>
-      </c>
-      <c r="B116" t="s">
-        <v>1091</v>
       </c>
       <c r="C116" t="s">
         <v>56</v>
       </c>
       <c r="D116" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E116" t="s">
         <v>1092</v>
       </c>
-      <c r="E116" t="s">
+      <c r="F116" t="s">
         <v>1093</v>
       </c>
-      <c r="F116" t="s">
+      <c r="G116" t="s">
         <v>1094</v>
       </c>
-      <c r="G116" t="s">
+      <c r="H116" s="2" t="s">
         <v>1095</v>
-      </c>
-      <c r="H116" s="2" t="s">
-        <v>1096</v>
       </c>
       <c r="I116" t="s">
         <v>8</v>
@@ -11912,10 +11909,10 @@
         <v>9</v>
       </c>
       <c r="K116" t="s">
+        <v>1096</v>
+      </c>
+      <c r="L116" t="s">
         <v>1097</v>
-      </c>
-      <c r="L116" t="s">
-        <v>1098</v>
       </c>
       <c r="M116" t="s">
         <v>324</v>
@@ -11945,28 +11942,28 @@
     </row>
     <row r="117" spans="1:20">
       <c r="A117" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B117" t="s">
         <v>1099</v>
-      </c>
-      <c r="B117" t="s">
-        <v>1100</v>
       </c>
       <c r="C117" t="s">
         <v>42</v>
       </c>
       <c r="D117" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E117" t="s">
         <v>1101</v>
       </c>
-      <c r="E117" t="s">
+      <c r="F117" t="s">
         <v>1102</v>
       </c>
-      <c r="F117" t="s">
+      <c r="G117" t="s">
         <v>1103</v>
       </c>
-      <c r="G117" t="s">
+      <c r="H117" s="2" t="s">
         <v>1104</v>
-      </c>
-      <c r="H117" s="2" t="s">
-        <v>1105</v>
       </c>
       <c r="I117" t="s">
         <v>14</v>
@@ -12008,28 +12005,28 @@
     </row>
     <row r="118" spans="1:20">
       <c r="A118" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B118" t="s">
         <v>1106</v>
-      </c>
-      <c r="B118" t="s">
-        <v>1107</v>
       </c>
       <c r="C118" t="s">
         <v>56</v>
       </c>
       <c r="D118" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E118" t="s">
         <v>1108</v>
       </c>
-      <c r="E118" t="s">
+      <c r="F118" t="s">
         <v>1109</v>
       </c>
-      <c r="F118" t="s">
+      <c r="G118" t="s">
         <v>1110</v>
       </c>
-      <c r="G118" t="s">
+      <c r="H118" s="2" t="s">
         <v>1111</v>
-      </c>
-      <c r="H118" s="2" t="s">
-        <v>1112</v>
       </c>
       <c r="I118" t="s">
         <v>8</v>
@@ -12041,7 +12038,7 @@
         <v>86</v>
       </c>
       <c r="L118" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="M118" t="s">
         <v>540</v>
@@ -12071,28 +12068,28 @@
     </row>
     <row r="119" spans="1:20">
       <c r="A119" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B119" t="s">
         <v>1114</v>
-      </c>
-      <c r="B119" t="s">
-        <v>1115</v>
       </c>
       <c r="C119" t="s">
         <v>2</v>
       </c>
       <c r="D119" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E119" t="s">
         <v>1116</v>
       </c>
-      <c r="E119" t="s">
+      <c r="F119" t="s">
         <v>1117</v>
       </c>
-      <c r="F119" t="s">
+      <c r="G119" t="s">
         <v>1118</v>
       </c>
-      <c r="G119" t="s">
+      <c r="H119" s="2" t="s">
         <v>1119</v>
-      </c>
-      <c r="H119" s="2" t="s">
-        <v>1120</v>
       </c>
       <c r="I119" t="s">
         <v>8</v>
@@ -12107,10 +12104,10 @@
         <v>11</v>
       </c>
       <c r="M119" t="s">
+        <v>1120</v>
+      </c>
+      <c r="N119" t="s">
         <v>1121</v>
-      </c>
-      <c r="N119" t="s">
-        <v>1122</v>
       </c>
       <c r="O119" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80551_sheffield", ".\export_data\inspection_reports\80551_sheffield")</f>
@@ -12134,28 +12131,28 @@
     </row>
     <row r="120" spans="1:20">
       <c r="A120" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B120" t="s">
         <v>1123</v>
-      </c>
-      <c r="B120" t="s">
-        <v>1124</v>
       </c>
       <c r="C120" t="s">
         <v>42</v>
       </c>
       <c r="D120" t="s">
+        <v>1124</v>
+      </c>
+      <c r="E120" t="s">
         <v>1125</v>
       </c>
-      <c r="E120" t="s">
+      <c r="F120" t="s">
         <v>1126</v>
       </c>
-      <c r="F120" t="s">
+      <c r="G120" t="s">
         <v>1127</v>
       </c>
-      <c r="G120" t="s">
+      <c r="H120" s="2" t="s">
         <v>1128</v>
-      </c>
-      <c r="H120" s="2" t="s">
-        <v>1129</v>
       </c>
       <c r="I120" t="s">
         <v>106</v>
@@ -12164,10 +12161,10 @@
         <v>48</v>
       </c>
       <c r="K120" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="L120" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="M120" t="s">
         <v>540</v>
@@ -12197,28 +12194,28 @@
     </row>
     <row r="121" spans="1:20">
       <c r="A121" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B121" t="s">
         <v>1131</v>
-      </c>
-      <c r="B121" t="s">
-        <v>1132</v>
       </c>
       <c r="C121" t="s">
         <v>100</v>
       </c>
       <c r="D121" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E121" t="s">
         <v>1133</v>
       </c>
-      <c r="E121" t="s">
+      <c r="F121" t="s">
         <v>1134</v>
       </c>
-      <c r="F121" t="s">
+      <c r="G121" t="s">
         <v>1135</v>
       </c>
-      <c r="G121" t="s">
+      <c r="H121" s="2" t="s">
         <v>1136</v>
-      </c>
-      <c r="H121" s="2" t="s">
-        <v>1137</v>
       </c>
       <c r="I121" t="s">
         <v>14</v>
@@ -12233,10 +12230,10 @@
         <v>472</v>
       </c>
       <c r="M121" t="s">
+        <v>1047</v>
+      </c>
+      <c r="N121" t="s">
         <v>1048</v>
-      </c>
-      <c r="N121" t="s">
-        <v>1049</v>
       </c>
       <c r="O121" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80553_slough", ".\export_data\inspection_reports\80553_slough")</f>
@@ -12260,28 +12257,28 @@
     </row>
     <row r="122" spans="1:20">
       <c r="A122" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B122" t="s">
         <v>1138</v>
-      </c>
-      <c r="B122" t="s">
-        <v>1139</v>
       </c>
       <c r="C122" t="s">
         <v>42</v>
       </c>
       <c r="D122" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E122" t="s">
         <v>1140</v>
       </c>
-      <c r="E122" t="s">
+      <c r="F122" t="s">
         <v>1141</v>
       </c>
-      <c r="F122" t="s">
+      <c r="G122" t="s">
         <v>1142</v>
       </c>
-      <c r="G122" t="s">
+      <c r="H122" s="2" t="s">
         <v>1143</v>
-      </c>
-      <c r="H122" s="2" t="s">
-        <v>1144</v>
       </c>
       <c r="I122" t="s">
         <v>191</v>
@@ -12290,7 +12287,7 @@
         <v>48</v>
       </c>
       <c r="K122" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="L122" t="s">
         <v>365</v>
@@ -12323,28 +12320,28 @@
     </row>
     <row r="123" spans="1:20">
       <c r="A123" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B123" t="s">
         <v>1146</v>
-      </c>
-      <c r="B123" t="s">
-        <v>1147</v>
       </c>
       <c r="C123" t="s">
         <v>18</v>
       </c>
       <c r="D123" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E123" t="s">
         <v>1148</v>
       </c>
-      <c r="E123" t="s">
+      <c r="F123" t="s">
         <v>1149</v>
       </c>
-      <c r="F123" t="s">
+      <c r="G123" t="s">
         <v>1150</v>
       </c>
-      <c r="G123" t="s">
+      <c r="H123" s="2" t="s">
         <v>1151</v>
-      </c>
-      <c r="H123" s="2" t="s">
-        <v>1152</v>
       </c>
       <c r="I123" t="s">
         <v>8</v>
@@ -12386,28 +12383,28 @@
     </row>
     <row r="124" spans="1:20">
       <c r="A124" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B124" t="s">
         <v>1153</v>
-      </c>
-      <c r="B124" t="s">
-        <v>1154</v>
       </c>
       <c r="C124" t="s">
         <v>18</v>
       </c>
       <c r="D124" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E124" t="s">
         <v>1155</v>
       </c>
-      <c r="E124" t="s">
+      <c r="F124" t="s">
         <v>1156</v>
       </c>
-      <c r="F124" t="s">
+      <c r="G124" t="s">
         <v>1157</v>
       </c>
-      <c r="G124" t="s">
+      <c r="H124" s="2" t="s">
         <v>1158</v>
-      </c>
-      <c r="H124" s="2" t="s">
-        <v>1159</v>
       </c>
       <c r="I124" t="s">
         <v>8</v>
@@ -12449,28 +12446,28 @@
     </row>
     <row r="125" spans="1:20">
       <c r="A125" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B125" t="s">
         <v>1160</v>
-      </c>
-      <c r="B125" t="s">
-        <v>1161</v>
       </c>
       <c r="C125" t="s">
         <v>294</v>
       </c>
       <c r="D125" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E125" t="s">
         <v>1162</v>
       </c>
-      <c r="E125" t="s">
+      <c r="F125" t="s">
         <v>1163</v>
       </c>
-      <c r="F125" t="s">
+      <c r="G125" t="s">
         <v>1164</v>
       </c>
-      <c r="G125" t="s">
+      <c r="H125" s="2" t="s">
         <v>1165</v>
-      </c>
-      <c r="H125" s="2" t="s">
-        <v>1166</v>
       </c>
       <c r="I125" t="s">
         <v>191</v>
@@ -12488,7 +12485,7 @@
         <v>530</v>
       </c>
       <c r="N125" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="O125" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80557_south tyneside", ".\export_data\inspection_reports\80557_south tyneside")</f>
@@ -12512,28 +12509,28 @@
     </row>
     <row r="126" spans="1:20">
       <c r="A126" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B126" t="s">
         <v>1168</v>
-      </c>
-      <c r="B126" t="s">
-        <v>1169</v>
       </c>
       <c r="C126" t="s">
         <v>100</v>
       </c>
       <c r="D126" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E126" t="s">
         <v>1170</v>
       </c>
-      <c r="E126" t="s">
+      <c r="F126" t="s">
         <v>1171</v>
       </c>
-      <c r="F126" t="s">
+      <c r="G126" t="s">
         <v>1172</v>
       </c>
-      <c r="G126" t="s">
+      <c r="H126" s="2" t="s">
         <v>1173</v>
-      </c>
-      <c r="H126" s="2" t="s">
-        <v>1174</v>
       </c>
       <c r="I126" t="s">
         <v>8</v>
@@ -12545,13 +12542,13 @@
         <v>394</v>
       </c>
       <c r="L126" t="s">
+        <v>1174</v>
+      </c>
+      <c r="M126" t="s">
         <v>1175</v>
       </c>
-      <c r="M126" t="s">
+      <c r="N126" t="s">
         <v>1176</v>
-      </c>
-      <c r="N126" t="s">
-        <v>1177</v>
       </c>
       <c r="O126" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80558_southampton", ".\export_data\inspection_reports\80558_southampton")</f>
@@ -12575,28 +12572,28 @@
     </row>
     <row r="127" spans="1:20">
       <c r="A127" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B127" t="s">
         <v>1178</v>
-      </c>
-      <c r="B127" t="s">
-        <v>1179</v>
       </c>
       <c r="C127" t="s">
         <v>31</v>
       </c>
       <c r="D127" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E127" t="s">
         <v>1180</v>
       </c>
-      <c r="E127" t="s">
+      <c r="F127" t="s">
         <v>1181</v>
       </c>
-      <c r="F127" t="s">
+      <c r="G127" t="s">
         <v>1182</v>
       </c>
-      <c r="G127" t="s">
+      <c r="H127" s="2" t="s">
         <v>1183</v>
-      </c>
-      <c r="H127" s="2" t="s">
-        <v>1184</v>
       </c>
       <c r="I127" t="s">
         <v>8</v>
@@ -12638,28 +12635,28 @@
     </row>
     <row r="128" spans="1:20">
       <c r="A128" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B128" t="s">
         <v>1185</v>
-      </c>
-      <c r="B128" t="s">
-        <v>1186</v>
       </c>
       <c r="C128" t="s">
         <v>56</v>
       </c>
       <c r="D128" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E128" t="s">
         <v>1187</v>
       </c>
-      <c r="E128" t="s">
+      <c r="F128" t="s">
         <v>1188</v>
       </c>
-      <c r="F128" t="s">
+      <c r="G128" t="s">
         <v>1189</v>
       </c>
-      <c r="G128" t="s">
+      <c r="H128" s="2" t="s">
         <v>1190</v>
-      </c>
-      <c r="H128" s="2" t="s">
-        <v>1191</v>
       </c>
       <c r="I128" t="s">
         <v>8</v>
@@ -12701,28 +12698,28 @@
     </row>
     <row r="129" spans="1:20">
       <c r="A129" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B129" t="s">
         <v>1192</v>
-      </c>
-      <c r="B129" t="s">
-        <v>1193</v>
       </c>
       <c r="C129" t="s">
         <v>42</v>
       </c>
       <c r="D129" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E129" t="s">
         <v>1194</v>
       </c>
-      <c r="E129" t="s">
+      <c r="F129" t="s">
         <v>1195</v>
       </c>
-      <c r="F129" t="s">
+      <c r="G129" t="s">
         <v>1196</v>
       </c>
-      <c r="G129" t="s">
+      <c r="H129" s="2" t="s">
         <v>1197</v>
-      </c>
-      <c r="H129" s="2" t="s">
-        <v>1198</v>
       </c>
       <c r="I129" t="s">
         <v>14</v>
@@ -12734,7 +12731,7 @@
         <v>202</v>
       </c>
       <c r="L129" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="M129" t="s">
         <v>324</v>
@@ -12764,28 +12761,28 @@
     </row>
     <row r="130" spans="1:20">
       <c r="A130" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B130" t="s">
         <v>1199</v>
-      </c>
-      <c r="B130" t="s">
-        <v>1200</v>
       </c>
       <c r="C130" t="s">
         <v>56</v>
       </c>
       <c r="D130" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E130" t="s">
         <v>1201</v>
       </c>
-      <c r="E130" t="s">
+      <c r="F130" t="s">
         <v>1202</v>
       </c>
-      <c r="F130" t="s">
+      <c r="G130" t="s">
         <v>1203</v>
       </c>
-      <c r="G130" t="s">
+      <c r="H130" s="2" t="s">
         <v>1204</v>
-      </c>
-      <c r="H130" s="2" t="s">
-        <v>1205</v>
       </c>
       <c r="I130" t="s">
         <v>14</v>
@@ -12803,7 +12800,7 @@
         <v>314</v>
       </c>
       <c r="N130" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="O130" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80562_stockport", ".\export_data\inspection_reports\80562_stockport")</f>
@@ -12827,28 +12824,28 @@
     </row>
     <row r="131" spans="1:20">
       <c r="A131" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B131" t="s">
         <v>1207</v>
-      </c>
-      <c r="B131" t="s">
-        <v>1208</v>
       </c>
       <c r="C131" t="s">
         <v>294</v>
       </c>
       <c r="D131" t="s">
+        <v>1208</v>
+      </c>
+      <c r="E131" t="s">
         <v>1209</v>
       </c>
-      <c r="E131" t="s">
+      <c r="F131" t="s">
         <v>1210</v>
       </c>
-      <c r="F131" t="s">
+      <c r="G131" t="s">
         <v>1211</v>
       </c>
-      <c r="G131" t="s">
+      <c r="H131" s="2" t="s">
         <v>1212</v>
-      </c>
-      <c r="H131" s="2" t="s">
-        <v>1213</v>
       </c>
       <c r="I131" t="s">
         <v>14</v>
@@ -12857,16 +12854,16 @@
         <v>48</v>
       </c>
       <c r="K131" t="s">
+        <v>1213</v>
+      </c>
+      <c r="L131" t="s">
         <v>1214</v>
       </c>
-      <c r="L131" t="s">
+      <c r="M131" t="s">
         <v>1215</v>
       </c>
-      <c r="M131" t="s">
+      <c r="N131" t="s">
         <v>1216</v>
-      </c>
-      <c r="N131" t="s">
-        <v>1217</v>
       </c>
       <c r="O131" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80563_stockton-on-tees", ".\export_data\inspection_reports\80563_stockton-on-tees")</f>
@@ -12890,28 +12887,28 @@
     </row>
     <row r="132" spans="1:20">
       <c r="A132" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B132" t="s">
         <v>1218</v>
-      </c>
-      <c r="B132" t="s">
-        <v>1219</v>
       </c>
       <c r="C132" t="s">
         <v>42</v>
       </c>
       <c r="D132" t="s">
+        <v>1219</v>
+      </c>
+      <c r="E132" t="s">
         <v>1220</v>
       </c>
-      <c r="E132" t="s">
+      <c r="F132" t="s">
         <v>1221</v>
       </c>
-      <c r="F132" t="s">
+      <c r="G132" t="s">
         <v>1222</v>
       </c>
-      <c r="G132" t="s">
+      <c r="H132" s="2" t="s">
         <v>1223</v>
-      </c>
-      <c r="H132" s="2" t="s">
-        <v>1224</v>
       </c>
       <c r="I132" t="s">
         <v>14</v>
@@ -12929,7 +12926,7 @@
         <v>314</v>
       </c>
       <c r="N132" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="O132" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80564_stoke-on-trent", ".\export_data\inspection_reports\80564_stoke-on-trent")</f>
@@ -12953,28 +12950,28 @@
     </row>
     <row r="133" spans="1:20">
       <c r="A133" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B133" t="s">
         <v>1225</v>
-      </c>
-      <c r="B133" t="s">
-        <v>1226</v>
       </c>
       <c r="C133" t="s">
         <v>31</v>
       </c>
       <c r="D133" t="s">
+        <v>1226</v>
+      </c>
+      <c r="E133" t="s">
         <v>1227</v>
       </c>
-      <c r="E133" t="s">
+      <c r="F133" t="s">
         <v>1228</v>
       </c>
-      <c r="F133" t="s">
+      <c r="G133" t="s">
         <v>1229</v>
       </c>
-      <c r="G133" t="s">
+      <c r="H133" s="2" t="s">
         <v>1230</v>
-      </c>
-      <c r="H133" s="2" t="s">
-        <v>1231</v>
       </c>
       <c r="I133" t="s">
         <v>14</v>
@@ -12992,7 +12989,7 @@
         <v>664</v>
       </c>
       <c r="N133" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="O133" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80565_suffolk", ".\export_data\inspection_reports\80565_suffolk")</f>
@@ -13016,28 +13013,28 @@
     </row>
     <row r="134" spans="1:20">
       <c r="A134" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B134" t="s">
         <v>1233</v>
-      </c>
-      <c r="B134" t="s">
-        <v>1234</v>
       </c>
       <c r="C134" t="s">
         <v>294</v>
       </c>
       <c r="D134" t="s">
+        <v>1234</v>
+      </c>
+      <c r="E134" t="s">
         <v>1235</v>
       </c>
-      <c r="E134" t="s">
+      <c r="F134" t="s">
         <v>1236</v>
       </c>
-      <c r="F134" t="s">
+      <c r="G134" t="s">
         <v>1237</v>
       </c>
-      <c r="G134" t="s">
+      <c r="H134" s="2" t="s">
         <v>1238</v>
-      </c>
-      <c r="H134" s="2" t="s">
-        <v>1239</v>
       </c>
       <c r="I134" t="s">
         <v>106</v>
@@ -13055,7 +13052,7 @@
         <v>346</v>
       </c>
       <c r="N134" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="O134" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80566_sunderland", ".\export_data\inspection_reports\80566_sunderland")</f>
@@ -13079,28 +13076,28 @@
     </row>
     <row r="135" spans="1:20">
       <c r="A135" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B135" t="s">
         <v>1241</v>
-      </c>
-      <c r="B135" t="s">
-        <v>1242</v>
       </c>
       <c r="C135" t="s">
         <v>100</v>
       </c>
       <c r="D135" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E135" t="s">
         <v>1243</v>
       </c>
-      <c r="E135" t="s">
+      <c r="F135" t="s">
         <v>1244</v>
       </c>
-      <c r="F135" t="s">
+      <c r="G135" t="s">
         <v>1245</v>
       </c>
-      <c r="G135" t="s">
+      <c r="H135" s="2" t="s">
         <v>1246</v>
-      </c>
-      <c r="H135" s="2" t="s">
-        <v>1247</v>
       </c>
       <c r="I135" t="s">
         <v>8</v>
@@ -13142,28 +13139,28 @@
     </row>
     <row r="136" spans="1:20">
       <c r="A136" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B136" t="s">
         <v>1248</v>
-      </c>
-      <c r="B136" t="s">
-        <v>1249</v>
       </c>
       <c r="C136" t="s">
         <v>18</v>
       </c>
       <c r="D136" t="s">
+        <v>1249</v>
+      </c>
+      <c r="E136" t="s">
         <v>1250</v>
       </c>
-      <c r="E136" t="s">
+      <c r="F136" t="s">
         <v>1251</v>
       </c>
-      <c r="F136" t="s">
+      <c r="G136" t="s">
         <v>1252</v>
       </c>
-      <c r="G136" t="s">
+      <c r="H136" s="2" t="s">
         <v>1253</v>
-      </c>
-      <c r="H136" s="2" t="s">
-        <v>1254</v>
       </c>
       <c r="I136" t="s">
         <v>191</v>
@@ -13205,28 +13202,28 @@
     </row>
     <row r="137" spans="1:20">
       <c r="A137" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B137" t="s">
         <v>1255</v>
-      </c>
-      <c r="B137" t="s">
-        <v>1256</v>
       </c>
       <c r="C137" t="s">
         <v>56</v>
       </c>
       <c r="D137" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E137" t="s">
         <v>1257</v>
       </c>
-      <c r="E137" t="s">
+      <c r="F137" t="s">
         <v>1258</v>
       </c>
-      <c r="F137" t="s">
+      <c r="G137" t="s">
         <v>1259</v>
       </c>
-      <c r="G137" t="s">
+      <c r="H137" s="2" t="s">
         <v>1260</v>
-      </c>
-      <c r="H137" s="2" t="s">
-        <v>1261</v>
       </c>
       <c r="I137" t="s">
         <v>191</v>
@@ -13244,7 +13241,7 @@
         <v>396</v>
       </c>
       <c r="N137" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="O137" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80569_tameside", ".\export_data\inspection_reports\80569_tameside")</f>
@@ -13268,28 +13265,28 @@
     </row>
     <row r="138" spans="1:20">
       <c r="A138" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B138" t="s">
         <v>1263</v>
-      </c>
-      <c r="B138" t="s">
-        <v>1264</v>
       </c>
       <c r="C138" t="s">
         <v>42</v>
       </c>
       <c r="D138" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E138" t="s">
         <v>1265</v>
       </c>
-      <c r="E138" t="s">
+      <c r="F138" t="s">
         <v>1266</v>
       </c>
-      <c r="F138" t="s">
+      <c r="G138" t="s">
         <v>1267</v>
       </c>
-      <c r="G138" t="s">
+      <c r="H138" s="2" t="s">
         <v>1268</v>
-      </c>
-      <c r="H138" s="2" t="s">
-        <v>1269</v>
       </c>
       <c r="I138" t="s">
         <v>106</v>
@@ -13301,7 +13298,7 @@
         <v>181</v>
       </c>
       <c r="L138" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="M138" t="s">
         <v>557</v>
@@ -13331,28 +13328,28 @@
     </row>
     <row r="139" spans="1:20">
       <c r="A139" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B139" t="s">
         <v>1271</v>
-      </c>
-      <c r="B139" t="s">
-        <v>1272</v>
       </c>
       <c r="C139" t="s">
         <v>31</v>
       </c>
       <c r="D139" t="s">
+        <v>1272</v>
+      </c>
+      <c r="E139" t="s">
         <v>1273</v>
       </c>
-      <c r="E139" t="s">
+      <c r="F139" t="s">
         <v>1274</v>
       </c>
-      <c r="F139" t="s">
+      <c r="G139" t="s">
         <v>1275</v>
       </c>
-      <c r="G139" t="s">
+      <c r="H139" s="2" t="s">
         <v>1276</v>
-      </c>
-      <c r="H139" s="2" t="s">
-        <v>1277</v>
       </c>
       <c r="I139" t="s">
         <v>106</v>
@@ -13364,13 +13361,13 @@
         <v>509</v>
       </c>
       <c r="L139" t="s">
+        <v>1277</v>
+      </c>
+      <c r="M139" t="s">
         <v>1278</v>
       </c>
-      <c r="M139" t="s">
+      <c r="N139" t="s">
         <v>1279</v>
-      </c>
-      <c r="N139" t="s">
-        <v>1280</v>
       </c>
       <c r="O139" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80571_thurrock", ".\export_data\inspection_reports\80571_thurrock")</f>
@@ -13394,28 +13391,28 @@
     </row>
     <row r="140" spans="1:20">
       <c r="A140" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B140" t="s">
         <v>1281</v>
-      </c>
-      <c r="B140" t="s">
-        <v>1282</v>
       </c>
       <c r="C140" t="s">
         <v>18</v>
       </c>
       <c r="D140" t="s">
+        <v>1282</v>
+      </c>
+      <c r="E140" t="s">
         <v>1283</v>
       </c>
-      <c r="E140" t="s">
+      <c r="F140" t="s">
         <v>1284</v>
       </c>
-      <c r="F140" t="s">
+      <c r="G140" t="s">
         <v>1285</v>
       </c>
-      <c r="G140" t="s">
+      <c r="H140" s="2" t="s">
         <v>1286</v>
-      </c>
-      <c r="H140" s="2" t="s">
-        <v>1287</v>
       </c>
       <c r="I140" t="s">
         <v>8</v>
@@ -13424,7 +13421,7 @@
         <v>48</v>
       </c>
       <c r="K140" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="L140" t="s">
         <v>856</v>
@@ -13433,7 +13430,7 @@
         <v>857</v>
       </c>
       <c r="N140" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="O140" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80572_torbay", ".\export_data\inspection_reports\80572_torbay")</f>
@@ -13457,28 +13454,28 @@
     </row>
     <row r="141" spans="1:20">
       <c r="A141" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B141" t="s">
         <v>1290</v>
-      </c>
-      <c r="B141" t="s">
-        <v>1291</v>
       </c>
       <c r="C141" t="s">
         <v>56</v>
       </c>
       <c r="D141" t="s">
+        <v>1291</v>
+      </c>
+      <c r="E141" t="s">
         <v>1292</v>
       </c>
-      <c r="E141" t="s">
+      <c r="F141" t="s">
         <v>1293</v>
       </c>
-      <c r="F141" t="s">
+      <c r="G141" t="s">
         <v>1294</v>
       </c>
-      <c r="G141" t="s">
+      <c r="H141" s="2" t="s">
         <v>1295</v>
-      </c>
-      <c r="H141" s="2" t="s">
-        <v>1296</v>
       </c>
       <c r="I141" t="s">
         <v>14</v>
@@ -13520,28 +13517,28 @@
     </row>
     <row r="142" spans="1:20">
       <c r="A142" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B142" t="s">
         <v>1297</v>
-      </c>
-      <c r="B142" t="s">
-        <v>1298</v>
       </c>
       <c r="C142" t="s">
         <v>42</v>
       </c>
       <c r="D142" t="s">
+        <v>1298</v>
+      </c>
+      <c r="E142" t="s">
         <v>1299</v>
       </c>
-      <c r="E142" t="s">
+      <c r="F142" t="s">
         <v>1300</v>
       </c>
-      <c r="F142" t="s">
+      <c r="G142" t="s">
         <v>1301</v>
       </c>
-      <c r="G142" t="s">
+      <c r="H142" s="2" t="s">
         <v>1302</v>
-      </c>
-      <c r="H142" s="2" t="s">
-        <v>1303</v>
       </c>
       <c r="I142" t="s">
         <v>106</v>
@@ -13583,28 +13580,28 @@
     </row>
     <row r="143" spans="1:20">
       <c r="A143" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B143" t="s">
         <v>1304</v>
-      </c>
-      <c r="B143" t="s">
-        <v>1305</v>
       </c>
       <c r="C143" t="s">
         <v>56</v>
       </c>
       <c r="D143" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E143" t="s">
         <v>1306</v>
       </c>
-      <c r="E143" t="s">
+      <c r="F143" t="s">
         <v>1307</v>
       </c>
-      <c r="F143" t="s">
+      <c r="G143" t="s">
         <v>1308</v>
       </c>
-      <c r="G143" t="s">
+      <c r="H143" s="2" t="s">
         <v>1309</v>
-      </c>
-      <c r="H143" s="2" t="s">
-        <v>1310</v>
       </c>
       <c r="I143" t="s">
         <v>8</v>
@@ -13622,7 +13619,7 @@
         <v>444</v>
       </c>
       <c r="N143" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="O143" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80575_warrington", ".\export_data\inspection_reports\80575_warrington")</f>
@@ -13646,28 +13643,28 @@
     </row>
     <row r="144" spans="1:20">
       <c r="A144" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B144" t="s">
         <v>1312</v>
-      </c>
-      <c r="B144" t="s">
-        <v>1313</v>
       </c>
       <c r="C144" t="s">
         <v>42</v>
       </c>
       <c r="D144" t="s">
+        <v>1313</v>
+      </c>
+      <c r="E144" t="s">
         <v>1314</v>
       </c>
-      <c r="E144" t="s">
+      <c r="F144" t="s">
         <v>1315</v>
       </c>
-      <c r="F144" t="s">
+      <c r="G144" t="s">
         <v>1316</v>
       </c>
-      <c r="G144" t="s">
+      <c r="H144" s="2" t="s">
         <v>1317</v>
-      </c>
-      <c r="H144" s="2" t="s">
-        <v>1318</v>
       </c>
       <c r="I144" t="s">
         <v>8</v>
@@ -13679,13 +13676,13 @@
         <v>202</v>
       </c>
       <c r="L144" t="s">
+        <v>1318</v>
+      </c>
+      <c r="M144" t="s">
         <v>1319</v>
       </c>
-      <c r="M144" t="s">
+      <c r="N144" t="s">
         <v>1320</v>
-      </c>
-      <c r="N144" t="s">
-        <v>1321</v>
       </c>
       <c r="O144" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80576_warwickshire", ".\export_data\inspection_reports\80576_warwickshire")</f>
@@ -13709,28 +13706,28 @@
     </row>
     <row r="145" spans="1:20">
       <c r="A145" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B145" t="s">
         <v>1322</v>
-      </c>
-      <c r="B145" t="s">
-        <v>1323</v>
       </c>
       <c r="C145" t="s">
         <v>100</v>
       </c>
       <c r="D145" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E145" t="s">
         <v>1324</v>
       </c>
-      <c r="E145" t="s">
+      <c r="F145" t="s">
         <v>1325</v>
       </c>
-      <c r="F145" t="s">
+      <c r="G145" t="s">
         <v>1326</v>
       </c>
-      <c r="G145" t="s">
+      <c r="H145" s="2" t="s">
         <v>1327</v>
-      </c>
-      <c r="H145" s="2" t="s">
-        <v>1328</v>
       </c>
       <c r="I145" t="s">
         <v>8</v>
@@ -13742,13 +13739,13 @@
         <v>118</v>
       </c>
       <c r="L145" t="s">
+        <v>1328</v>
+      </c>
+      <c r="M145" t="s">
         <v>1329</v>
       </c>
-      <c r="M145" t="s">
+      <c r="N145" t="s">
         <v>1330</v>
-      </c>
-      <c r="N145" t="s">
-        <v>1331</v>
       </c>
       <c r="O145" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80577_west berkshire", ".\export_data\inspection_reports\80577_west berkshire")</f>
@@ -13772,28 +13769,28 @@
     </row>
     <row r="146" spans="1:20">
       <c r="A146" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B146" t="s">
         <v>1332</v>
-      </c>
-      <c r="B146" t="s">
-        <v>1333</v>
       </c>
       <c r="C146" t="s">
         <v>306</v>
       </c>
       <c r="D146" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E146" t="s">
         <v>1334</v>
       </c>
-      <c r="E146" t="s">
+      <c r="F146" t="s">
         <v>1335</v>
       </c>
-      <c r="F146" t="s">
+      <c r="G146" t="s">
         <v>1336</v>
       </c>
-      <c r="G146" t="s">
+      <c r="H146" s="2" t="s">
         <v>1337</v>
-      </c>
-      <c r="H146" s="2" t="s">
-        <v>1338</v>
       </c>
       <c r="I146" t="s">
         <v>14</v>
@@ -13805,13 +13802,13 @@
         <v>202</v>
       </c>
       <c r="L146" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="M146" t="s">
+        <v>921</v>
+      </c>
+      <c r="N146" t="s">
         <v>922</v>
-      </c>
-      <c r="N146" t="s">
-        <v>923</v>
       </c>
       <c r="O146" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\2637548_west northamptonshire", ".\export_data\inspection_reports\2637548_west northamptonshire")</f>
@@ -13835,28 +13832,28 @@
     </row>
     <row r="147" spans="1:20">
       <c r="A147" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B147" t="s">
         <v>1339</v>
-      </c>
-      <c r="B147" t="s">
-        <v>1340</v>
       </c>
       <c r="C147" t="s">
         <v>100</v>
       </c>
       <c r="D147" t="s">
+        <v>1340</v>
+      </c>
+      <c r="E147" t="s">
         <v>1341</v>
       </c>
-      <c r="E147" t="s">
+      <c r="F147" t="s">
         <v>1342</v>
       </c>
-      <c r="F147" t="s">
+      <c r="G147" t="s">
         <v>1343</v>
       </c>
-      <c r="G147" t="s">
+      <c r="H147" s="2" t="s">
         <v>1344</v>
-      </c>
-      <c r="H147" s="2" t="s">
-        <v>1345</v>
       </c>
       <c r="I147" t="s">
         <v>14</v>
@@ -13865,7 +13862,7 @@
         <v>48</v>
       </c>
       <c r="K147" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="L147" t="s">
         <v>575</v>
@@ -13874,7 +13871,7 @@
         <v>576</v>
       </c>
       <c r="N147" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="O147" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80578_west sussex", ".\export_data\inspection_reports\80578_west sussex")</f>
@@ -13898,10 +13895,10 @@
     </row>
     <row r="148" spans="1:20">
       <c r="A148" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B148" t="s">
         <v>1347</v>
-      </c>
-      <c r="B148" t="s">
-        <v>1348</v>
       </c>
       <c r="C148" t="s">
         <v>56</v>
@@ -13910,16 +13907,16 @@
         <v>284</v>
       </c>
       <c r="E148" t="s">
+        <v>1348</v>
+      </c>
+      <c r="F148" t="s">
         <v>1349</v>
       </c>
-      <c r="F148" t="s">
+      <c r="G148" t="s">
         <v>1350</v>
       </c>
-      <c r="G148" t="s">
+      <c r="H148" s="2" t="s">
         <v>1351</v>
-      </c>
-      <c r="H148" s="2" t="s">
-        <v>1352</v>
       </c>
       <c r="I148" t="s">
         <v>8</v>
@@ -13928,7 +13925,7 @@
         <v>48</v>
       </c>
       <c r="K148" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="L148" t="s">
         <v>556</v>
@@ -13961,28 +13958,28 @@
     </row>
     <row r="149" spans="1:20">
       <c r="A149" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B149" t="s">
         <v>1353</v>
-      </c>
-      <c r="B149" t="s">
-        <v>1354</v>
       </c>
       <c r="C149" t="s">
         <v>56</v>
       </c>
       <c r="D149" t="s">
+        <v>1354</v>
+      </c>
+      <c r="E149" t="s">
         <v>1355</v>
       </c>
-      <c r="E149" t="s">
+      <c r="F149" t="s">
         <v>1356</v>
       </c>
-      <c r="F149" t="s">
+      <c r="G149" t="s">
         <v>1357</v>
       </c>
-      <c r="G149" t="s">
+      <c r="H149" s="2" t="s">
         <v>1358</v>
-      </c>
-      <c r="H149" s="2" t="s">
-        <v>1359</v>
       </c>
       <c r="I149" t="s">
         <v>14</v>
@@ -13991,7 +13988,7 @@
         <v>48</v>
       </c>
       <c r="K149" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="L149" t="s">
         <v>489</v>
@@ -14024,28 +14021,28 @@
     </row>
     <row r="150" spans="1:20">
       <c r="A150" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B150" t="s">
         <v>1361</v>
-      </c>
-      <c r="B150" t="s">
-        <v>1362</v>
       </c>
       <c r="C150" t="s">
         <v>18</v>
       </c>
       <c r="D150" t="s">
+        <v>1362</v>
+      </c>
+      <c r="E150" t="s">
         <v>1363</v>
       </c>
-      <c r="E150" t="s">
+      <c r="F150" t="s">
         <v>1364</v>
       </c>
-      <c r="F150" t="s">
+      <c r="G150" t="s">
         <v>1365</v>
       </c>
-      <c r="G150" t="s">
+      <c r="H150" s="2" t="s">
         <v>1366</v>
-      </c>
-      <c r="H150" s="2" t="s">
-        <v>1367</v>
       </c>
       <c r="I150" t="s">
         <v>106</v>
@@ -14057,13 +14054,13 @@
         <v>405</v>
       </c>
       <c r="L150" t="s">
+        <v>1367</v>
+      </c>
+      <c r="M150" t="s">
         <v>1368</v>
       </c>
-      <c r="M150" t="s">
+      <c r="N150" t="s">
         <v>1369</v>
-      </c>
-      <c r="N150" t="s">
-        <v>1370</v>
       </c>
       <c r="O150" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80580_wiltshire", ".\export_data\inspection_reports\80580_wiltshire")</f>
@@ -14087,28 +14084,28 @@
     </row>
     <row r="151" spans="1:20">
       <c r="A151" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B151" t="s">
         <v>1371</v>
-      </c>
-      <c r="B151" t="s">
-        <v>1372</v>
       </c>
       <c r="C151" t="s">
         <v>56</v>
       </c>
       <c r="D151" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E151" t="s">
         <v>1373</v>
       </c>
-      <c r="E151" t="s">
+      <c r="F151" t="s">
         <v>1374</v>
       </c>
-      <c r="F151" t="s">
+      <c r="G151" t="s">
         <v>1375</v>
       </c>
-      <c r="G151" t="s">
+      <c r="H151" s="2" t="s">
         <v>1376</v>
-      </c>
-      <c r="H151" s="2" t="s">
-        <v>1377</v>
       </c>
       <c r="I151" t="s">
         <v>14</v>
@@ -14120,13 +14117,13 @@
         <v>192</v>
       </c>
       <c r="L151" t="s">
+        <v>1377</v>
+      </c>
+      <c r="M151" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N151" t="s">
         <v>1378</v>
-      </c>
-      <c r="M151" t="s">
-        <v>1369</v>
-      </c>
-      <c r="N151" t="s">
-        <v>1379</v>
       </c>
       <c r="O151" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80581_wirral", ".\export_data\inspection_reports\80581_wirral")</f>
@@ -14150,28 +14147,28 @@
     </row>
     <row r="152" spans="1:20">
       <c r="A152" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B152" t="s">
         <v>1380</v>
-      </c>
-      <c r="B152" t="s">
-        <v>1381</v>
       </c>
       <c r="C152" t="s">
         <v>100</v>
       </c>
       <c r="D152" t="s">
+        <v>1381</v>
+      </c>
+      <c r="E152" t="s">
         <v>1382</v>
       </c>
-      <c r="E152" t="s">
+      <c r="F152" t="s">
         <v>1383</v>
       </c>
-      <c r="F152" t="s">
+      <c r="G152" t="s">
         <v>1384</v>
       </c>
-      <c r="G152" t="s">
+      <c r="H152" s="2" t="s">
         <v>1385</v>
-      </c>
-      <c r="H152" s="2" t="s">
-        <v>1386</v>
       </c>
       <c r="I152" t="s">
         <v>14</v>
@@ -14183,13 +14180,13 @@
         <v>394</v>
       </c>
       <c r="L152" t="s">
+        <v>1214</v>
+      </c>
+      <c r="M152" t="s">
         <v>1215</v>
       </c>
-      <c r="M152" t="s">
+      <c r="N152" t="s">
         <v>1216</v>
-      </c>
-      <c r="N152" t="s">
-        <v>1217</v>
       </c>
       <c r="O152" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80582_wokingham", ".\export_data\inspection_reports\80582_wokingham")</f>
@@ -14213,28 +14210,28 @@
     </row>
     <row r="153" spans="1:20">
       <c r="A153" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B153" t="s">
         <v>1387</v>
-      </c>
-      <c r="B153" t="s">
-        <v>1388</v>
       </c>
       <c r="C153" t="s">
         <v>42</v>
       </c>
       <c r="D153" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E153" t="s">
         <v>1389</v>
       </c>
-      <c r="E153" t="s">
+      <c r="F153" t="s">
         <v>1390</v>
       </c>
-      <c r="F153" t="s">
+      <c r="G153" t="s">
         <v>1391</v>
       </c>
-      <c r="G153" t="s">
+      <c r="H153" s="2" t="s">
         <v>1392</v>
-      </c>
-      <c r="H153" s="2" t="s">
-        <v>1393</v>
       </c>
       <c r="I153" t="s">
         <v>8</v>
@@ -14243,16 +14240,16 @@
         <v>9</v>
       </c>
       <c r="K153" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="L153" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="M153" t="s">
         <v>857</v>
       </c>
       <c r="N153" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="O153" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80583_wolverhampton", ".\export_data\inspection_reports\80583_wolverhampton")</f>
@@ -14276,28 +14273,28 @@
     </row>
     <row r="154" spans="1:20">
       <c r="A154" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B154" t="s">
         <v>1395</v>
-      </c>
-      <c r="B154" t="s">
-        <v>1396</v>
       </c>
       <c r="C154" t="s">
         <v>42</v>
       </c>
       <c r="D154" t="s">
+        <v>1396</v>
+      </c>
+      <c r="E154" t="s">
         <v>1397</v>
       </c>
-      <c r="E154" t="s">
+      <c r="F154" t="s">
         <v>1398</v>
       </c>
-      <c r="F154" t="s">
+      <c r="G154" t="s">
         <v>1399</v>
       </c>
-      <c r="G154" t="s">
+      <c r="H154" s="2" t="s">
         <v>1400</v>
-      </c>
-      <c r="H154" s="2" t="s">
-        <v>1401</v>
       </c>
       <c r="I154" t="s">
         <v>8</v>
@@ -14309,13 +14306,13 @@
         <v>181</v>
       </c>
       <c r="L154" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="M154" t="s">
+        <v>1401</v>
+      </c>
+      <c r="N154" t="s">
         <v>1402</v>
-      </c>
-      <c r="N154" t="s">
-        <v>1403</v>
       </c>
       <c r="O154" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80584_worcestershire", ".\export_data\inspection_reports\80584_worcestershire")</f>

</xml_diff>